<commit_message>
Week 3-1 introduction to css utility classes
</commit_message>
<xml_diff>
--- a/@cheetsheets/css_properties.xlsx
+++ b/@cheetsheets/css_properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\@dev\netit-webdev-js\@cheetsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{444BF266-E6FC-459F-8335-8ABB5AA43DA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3CA510-99D0-46A0-86C7-438274DD2F22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{574DD0F0-4A54-4DA8-911E-95E3FDCC618D}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
-  <si>
-    <t>цветове</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>background-color</t>
   </si>
@@ -36,9 +33,6 @@
     <t>color</t>
   </si>
   <si>
-    <t>измерения</t>
-  </si>
-  <si>
     <t>border</t>
   </si>
   <si>
@@ -105,13 +99,25 @@
     <t>DIMENTION VALUE</t>
   </si>
   <si>
-    <t>текст и шрифт стилове</t>
-  </si>
-  <si>
     <t>text-decoration</t>
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>стилове за цветове</t>
+  </si>
+  <si>
+    <t>стилове за измерения</t>
+  </si>
+  <si>
+    <t>стилове за текст и шрифт</t>
+  </si>
+  <si>
+    <t>font-size</t>
+  </si>
+  <si>
+    <t>font-weight</t>
   </si>
 </sst>
 </file>
@@ -174,15 +180,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACB29B8-5F3C-4E5B-B619-06969D261E6A}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,199 +516,212 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3"/>
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
+      <c r="A7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
+      <c r="A8" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
+      <c r="A9" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
+      <c r="A11" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
+      <c r="A12" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
+      <c r="A13" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
+      <c r="A14" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
+      <c r="A16" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
+      <c r="A17" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
+      <c r="A18" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
+      <c r="A22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>